<commit_message>
Avancament MEP Frame 90%
</commit_message>
<xml_diff>
--- a/FR_Frame_Body/FR_A0100 (Frame)/Frame_Production/MEP/Suivi_Plans_Frame_2020.xlsx
+++ b/FR_Frame_Body/FR_A0100 (Frame)/Frame_Production/MEP/Suivi_Plans_Frame_2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Calixthe\Desktop\EPSA\STUF-2020\FR_Frame_Body\FR_A0100 (Frame)\Frame_Production\MEP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C6BC66-3A5B-4351-827F-7A5EA62FEBA3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B82F3F-93FA-4A09-BF34-E3E6DFE60A24}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{09D4FF9D-7721-445A-9DC3-1C3BC7278DAC}"/>
+    <workbookView xWindow="2568" yWindow="3300" windowWidth="17280" windowHeight="9060" xr2:uid="{09D4FF9D-7721-445A-9DC3-1C3BC7278DAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>Suivi Plans Frame</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Floor</t>
   </si>
   <si>
-    <t>Frame Vue de dos</t>
-  </si>
-  <si>
     <t>N°</t>
   </si>
   <si>
@@ -82,6 +79,36 @@
   </si>
   <si>
     <t>Oui</t>
+  </si>
+  <si>
+    <t>Under Frame</t>
+  </si>
+  <si>
+    <t>Bracing à découper</t>
+  </si>
+  <si>
+    <t>Frame Top View</t>
+  </si>
+  <si>
+    <t>20_G_FR_A0100_#07</t>
+  </si>
+  <si>
+    <t>20_G_FR_A0100_201</t>
+  </si>
+  <si>
+    <t>20_G_FR_A0100_202</t>
+  </si>
+  <si>
+    <t>Front Hoop</t>
+  </si>
+  <si>
+    <t>Main Hoop</t>
+  </si>
+  <si>
+    <t>MJT</t>
+  </si>
+  <si>
+    <t>Cellule Arrière</t>
   </si>
 </sst>
 </file>
@@ -162,25 +189,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -496,15 +509,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A461B67-D253-4F3E-8E7E-8ECD68298490}">
   <dimension ref="B3:G19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.5546875" style="1"/>
     <col min="2" max="2" width="19.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
@@ -536,7 +549,7 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>1</v>
@@ -553,31 +566,33 @@
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>7</v>
@@ -588,52 +603,82 @@
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="B17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="B18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="F18" s="2"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="B19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="F19" s="2"/>
     </row>
   </sheetData>
@@ -641,7 +686,7 @@
     <mergeCell ref="D3:G6"/>
   </mergeCells>
   <conditionalFormatting sqref="D11:D19 F11:F19">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Oui">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Oui">
       <formula>NOT(ISERROR(SEARCH("Oui",D11)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fin des MEP Frame
Manque plus que la vérification et les dernières modifs
</commit_message>
<xml_diff>
--- a/FR_Frame_Body/FR_A0100 (Frame)/Frame_Production/MEP/Suivi_Plans_Frame_2020.xlsx
+++ b/FR_Frame_Body/FR_A0100 (Frame)/Frame_Production/MEP/Suivi_Plans_Frame_2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Calixthe\Desktop\EPSA\STUF-2020\FR_Frame_Body\FR_A0100 (Frame)\Frame_Production\MEP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B82F3F-93FA-4A09-BF34-E3E6DFE60A24}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4EBD527-075B-4322-906C-ADE4265C9F05}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2568" yWindow="3300" windowWidth="17280" windowHeight="9060" xr2:uid="{09D4FF9D-7721-445A-9DC3-1C3BC7278DAC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{09D4FF9D-7721-445A-9DC3-1C3BC7278DAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>Suivi Plans Frame</t>
   </si>
@@ -109,6 +109,12 @@
   </si>
   <si>
     <t>Cellule Arrière</t>
+  </si>
+  <si>
+    <t>Commentaires</t>
+  </si>
+  <si>
+    <t>Oui,</t>
   </si>
 </sst>
 </file>
@@ -171,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -185,11 +191,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -509,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A461B67-D253-4F3E-8E7E-8ECD68298490}">
   <dimension ref="B3:G19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -518,7 +534,9 @@
     <col min="1" max="1" width="11.5546875" style="1"/>
     <col min="2" max="2" width="19.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="11.5546875" style="1"/>
+    <col min="4" max="5" width="11.5546875" style="1"/>
+    <col min="6" max="6" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
@@ -561,6 +579,9 @@
         <v>4</v>
       </c>
       <c r="F10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -576,6 +597,7 @@
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
@@ -589,6 +611,7 @@
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
@@ -597,9 +620,12 @@
       <c r="C13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
@@ -613,6 +639,7 @@
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
@@ -621,9 +648,12 @@
       <c r="C15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="2"/>
+      <c r="D15" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
@@ -637,8 +667,9 @@
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>19</v>
       </c>
@@ -650,8 +681,9 @@
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>20</v>
       </c>
@@ -665,8 +697,9 @@
         <v>24</v>
       </c>
       <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>21</v>
       </c>
@@ -680,14 +713,20 @@
         <v>24</v>
       </c>
       <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D3:G6"/>
   </mergeCells>
   <conditionalFormatting sqref="D11:D19 F11:F19">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Oui">
+      <formula>NOT(ISERROR(SEARCH("Oui",D11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11:G19">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Oui">
-      <formula>NOT(ISERROR(SEARCH("Oui",D11)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Oui",G11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>